<commit_message>
Add daos to load regions, countries, observations, indicators, subindexes and components, and its test
</commit_message>
<xml_diff>
--- a/src/main/resources/computex/example.xlsx
+++ b/src/main/resources/computex/example.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nacho\Web_Foundation_Index\wiFetcher\src\main\resources\computex\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="17115" windowHeight="7935" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19950" windowHeight="7905" tabRatio="554" firstSheet="20" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -13,22 +18,36 @@
     <sheet name="C-RAW" sheetId="7" r:id="rId4"/>
     <sheet name="D-Raw" sheetId="8" r:id="rId5"/>
     <sheet name="Q1" sheetId="9" r:id="rId6"/>
-    <sheet name="Q2" sheetId="10" r:id="rId7"/>
-    <sheet name="A-Imputed" sheetId="4" r:id="rId8"/>
-    <sheet name="C-IMPUTED" sheetId="11" r:id="rId9"/>
-    <sheet name="A-NORMALISED" sheetId="5" r:id="rId10"/>
+    <sheet name="Q1-Normalized" sheetId="17" r:id="rId7"/>
+    <sheet name="Q2" sheetId="10" r:id="rId8"/>
+    <sheet name="Q2-Normalized" sheetId="18" r:id="rId9"/>
+    <sheet name="A-Imputed" sheetId="4" r:id="rId10"/>
+    <sheet name="B-Imputed" sheetId="12" r:id="rId11"/>
+    <sheet name="C-Imputed" sheetId="11" r:id="rId12"/>
+    <sheet name="D-Imputed" sheetId="13" r:id="rId13"/>
+    <sheet name="A-Normalized" sheetId="5" r:id="rId14"/>
+    <sheet name="B-Normalized" sheetId="15" r:id="rId15"/>
+    <sheet name="C-Normalized" sheetId="14" r:id="rId16"/>
+    <sheet name="D-Normalized" sheetId="16" r:id="rId17"/>
+    <sheet name="Indicators-Normalized" sheetId="21" r:id="rId18"/>
+    <sheet name="Indicators-Incremented" sheetId="24" r:id="rId19"/>
+    <sheet name="Indicators-Weighted" sheetId="25" r:id="rId20"/>
+    <sheet name="Components-Weighted" sheetId="22" r:id="rId21"/>
+    <sheet name="Subindex-Weighted" sheetId="26" r:id="rId22"/>
+    <sheet name="Index-Weighted" sheetId="27" r:id="rId23"/>
+    <sheet name="Rankings" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="countries">Metadata!$A$14:$A$249</definedName>
     <definedName name="datatype">Metadata!$A$5:$A$7</definedName>
     <definedName name="indicators">Metadata!$A$252:$A$336</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="285">
   <si>
     <t>Raw</t>
   </si>
@@ -36,9 +55,6 @@
     <t>The original data as found on the source</t>
   </si>
   <si>
-    <t>Inputed</t>
-  </si>
-  <si>
     <t>Data including the gaps, see also inputed method</t>
   </si>
   <si>
@@ -51,18 +67,6 @@
     <t>Inputed method</t>
   </si>
   <si>
-    <t>average</t>
-  </si>
-  <si>
-    <t>missing values inputed by average</t>
-  </si>
-  <si>
-    <t>projectXXX</t>
-  </si>
-  <si>
-    <t>inputed by XXX projection</t>
-  </si>
-  <si>
     <t>Normalised country names</t>
   </si>
   <si>
@@ -822,14 +826,92 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>TODO</t>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Notice that the z-score formula used here is different because indicator B is Low</t>
+  </si>
+  <si>
+    <t>Components</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>DQ1</t>
+  </si>
+  <si>
+    <t>Subindex</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>ABQ2</t>
+  </si>
+  <si>
+    <t>CDQ1</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C </t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Composite</t>
+  </si>
+  <si>
+    <t>Indicators Type</t>
+  </si>
+  <si>
+    <t>HighLow</t>
+  </si>
+  <si>
+    <t>Average Growth</t>
+  </si>
+  <si>
+    <t>Missing values as Average of previous and next</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>AverageGrowth</t>
+  </si>
+  <si>
+    <t>Imputed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -877,13 +959,37 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -914,8 +1020,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -932,11 +1044,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -950,25 +1073,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7AB800"/>
+      <color rgb="FF008000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1278,31 +1424,31 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:C257"/>
+  <dimension ref="A2:C272"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A250" sqref="A250"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.125" customWidth="1"/>
-    <col min="2" max="2" width="42.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="38.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="B2" s="11"/>
+      <c r="A2" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="26"/>
       <c r="C2" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,1260 +1460,1378 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
+      <c r="A10" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
+      <c r="A11" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A241" t="s">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A243" t="s">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
+    <row r="251" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A246" t="s">
+      <c r="B251" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>253</v>
+      </c>
+      <c r="B252" t="s">
+        <v>262</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>254</v>
+      </c>
+      <c r="B253" t="s">
+        <v>263</v>
+      </c>
+      <c r="C253">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>255</v>
+      </c>
+      <c r="B254" t="s">
+        <v>262</v>
+      </c>
+      <c r="C254">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>256</v>
+      </c>
+      <c r="B255" t="s">
+        <v>262</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A247" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A249" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A255" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A256" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B256" t="s">
+        <v>262</v>
+      </c>
+      <c r="C256">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
+        <v>257</v>
+      </c>
+      <c r="B257" t="s">
         <v>262</v>
+      </c>
+      <c r="C257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>266</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>257</v>
+      </c>
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>275</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>267</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>272</v>
+      </c>
+      <c r="B267">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>273</v>
+      </c>
+      <c r="B268">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2579,99 +2843,165 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="5"/>
     <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
+    <col min="3" max="3" width="11.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>256</v>
-      </c>
       <c r="C3" s="6">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D3" s="6">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="E3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="F3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="G3" s="6">
         <v>2011</v>
       </c>
-      <c r="H3" s="6">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <f>AVERAGE(C6,E6)</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>datatype</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2683,23 +3013,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -2713,50 +3043,87 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
         <v>3</v>
-      </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5">
-        <v>5</v>
-      </c>
-      <c r="E7" s="14">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2776,12 +3143,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2793,15 +3160,1084 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <f>AVERAGE(C6,E6)</f>
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>8</v>
+      </c>
+      <c r="E7" s="16">
+        <f>D7*AVERAGE(D7/C7)</f>
+        <v>10.666666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(C5:C7)</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="D9" s="13">
+        <f>AVERAGE(D5:D7)</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13">
+        <f>AVERAGE(E5:E7)</f>
+        <v>6.5555555555555545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1.1547005383792526</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="E10" s="5">
+        <f>STDEV(E5:E7)</f>
+        <v>3.8634085890474927</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
+      <c r="E7" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D9" s="5">
+        <f>AVERAGE(D5:D7)</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <f>AVERAGE(E5:E7)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1.154700538379251</v>
+      </c>
+      <c r="D10" s="5">
+        <f>STDEV(D5:D7)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="E10" s="19">
+        <f>STDEV(E5:E7)</f>
+        <v>2.309401076758502</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('A-Imputed'!C$5-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('A-Imputed'!D$5-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('A-Imputed'!E$5-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('A-Imputed'!C$6-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('A-Imputed'!D$6-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('A-Imputed'!E$6-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('A-Imputed'!C$7-'A-Imputed'!C$9)/'A-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('A-Imputed'!D$7-'A-Imputed'!D$9)/'A-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('A-Imputed'!E$7-'A-Imputed'!E$9)/'A-Imputed'!E$10</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$5)/'B-Imputed'!C$10</f>
+        <v>-1</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$5)/'B-Imputed'!D$10</f>
+        <v>-1</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$5)/'B-Imputed'!E$10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$6)/'B-Imputed'!C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$6)/'B-Imputed'!D$10</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$6)/'B-Imputed'!E$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('B-Imputed'!C$9-'B-Imputed'!C$7)/'B-Imputed'!C$10</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('B-Imputed'!D$9-'B-Imputed'!D$7)/'B-Imputed'!D$10</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('B-Imputed'!E$9-'B-Imputed'!E$7)/'B-Imputed'!E$10</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('C-Imputed'!C$5-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('C-Imputed'!D$5-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('C-Imputed'!E$5-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.92031569366888055</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('C-Imputed'!C$6-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>-0.57735026918962551</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('C-Imputed'!D$6-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>-0.57735026918962584</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('C-Imputed'!E$6-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>-0.14379932713576235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('C-Imputed'!C$7-'C-Imputed'!C$9)/'C-Imputed'!C$10</f>
+        <v>1.1547005383792501</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('C-Imputed'!D$7-'C-Imputed'!D$9)/'C-Imputed'!D$10</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('C-Imputed'!E$7-'C-Imputed'!E$9)/'C-Imputed'!E$10</f>
+        <v>1.0641150208046437</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('D-Imputed'!C$5-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D5" s="5">
+        <f>('D-Imputed'!D$5-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E5" s="5">
+        <f>('D-Imputed'!E$5-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('D-Imputed'!C$6-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="D6" s="5">
+        <f>('D-Imputed'!D$6-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>-1.1547005383792517</v>
+      </c>
+      <c r="E6" s="5">
+        <f>('D-Imputed'!E$6-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>-1.1547005383792521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('D-Imputed'!C$7-'D-Imputed'!C$9)/'D-Imputed'!C$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="D7" s="5">
+        <f>('D-Imputed'!D$7-'D-Imputed'!D$9)/'D-Imputed'!D$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="E7" s="5">
+        <f>('D-Imputed'!E$7-'D-Imputed'!E$9)/'D-Imputed'!E$10</f>
+        <v>0.57735026918962584</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="5">
+        <f>'A-Normalized'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <f>'B-Normalized'!E$5</f>
+        <v>-1</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'Q2-Normalized'!C$5</f>
+        <v>1.1208970766356094</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'C-Normalized'!E$5</f>
+        <v>-0.92031569366888055</v>
+      </c>
+      <c r="F2" s="5">
+        <f>'D-Normalized'!E$5</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G2" s="5">
+        <f>'Q1-Normalized'!C$5</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5">
+        <f>'A-Normalized'!E6</f>
+        <v>-1</v>
+      </c>
+      <c r="C3" s="5">
+        <f>'B-Normalized'!E6</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <f>'Q2-Normalized'!C$6</f>
+        <v>-0.80064076902543546</v>
+      </c>
+      <c r="E3" s="5">
+        <f>'C-Normalized'!E6</f>
+        <v>-0.14379932713576235</v>
+      </c>
+      <c r="F3" s="5">
+        <f>'D-Normalized'!E6</f>
+        <v>-1.1547005383792521</v>
+      </c>
+      <c r="G3" s="5">
+        <f>'Q1-Normalized'!C$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'A-Normalized'!E7</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'B-Normalized'!E7</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'Q2-Normalized'!C$7</f>
+        <v>-0.32025630761017432</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'C-Normalized'!E7</f>
+        <v>1.0641150208046437</v>
+      </c>
+      <c r="F4" s="5">
+        <f>'D-Normalized'!E7</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G4" s="5">
+        <f>'Q1-Normalized'!C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A74:A338 A2:A5">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$252:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="5">
+        <f>'Indicators-Normalized'!B2+8</f>
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
+        <f>'Indicators-Normalized'!C2+8</f>
+        <v>7</v>
+      </c>
+      <c r="D2" s="5">
+        <f>'Indicators-Normalized'!D2+8</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E2" s="5">
+        <f>'Indicators-Normalized'!E2+8</f>
+        <v>7.079684306331119</v>
+      </c>
+      <c r="F2" s="5">
+        <f>'Indicators-Normalized'!F2+8</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G2" s="5">
+        <f>'Indicators-Normalized'!G2+8</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="5">
+        <f>'Indicators-Normalized'!B3+8</f>
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <f>'Indicators-Normalized'!C3+8</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <f>'Indicators-Normalized'!D3+8</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E3" s="5">
+        <f>'Indicators-Normalized'!E3+8</f>
+        <v>7.8562006728642375</v>
+      </c>
+      <c r="F3" s="5">
+        <f>'Indicators-Normalized'!F3+8</f>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G3" s="5">
+        <f>'Indicators-Normalized'!G3+8</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="5">
+        <f>'Indicators-Normalized'!B4+8</f>
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <f>'Indicators-Normalized'!C4+8</f>
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
+        <f>'Indicators-Normalized'!D4+8</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E4" s="5">
+        <f>'Indicators-Normalized'!E4+8</f>
+        <v>9.0641150208046444</v>
+      </c>
+      <c r="F4" s="5">
+        <f>'Indicators-Normalized'!F4+8</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G4" s="5">
+        <f>'Indicators-Normalized'!G4+8</f>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A73:A337 A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$252:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -2809,7 +4245,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -2823,15 +4259,681 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="20">
+        <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B2*Metadata!C252)</f>
+        <v>8</v>
+      </c>
+      <c r="C2" s="20">
+        <f>IF(Metadata!C253&gt;0,'Indicators-Incremented'!C2*Metadata!C253)</f>
+        <v>3.5</v>
+      </c>
+      <c r="D2" s="20">
+        <f>IF(Metadata!C257&gt;0,'Indicators-Incremented'!D2*Metadata!C257)</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="E2" s="20">
+        <f>IF(Metadata!C254&gt;0,'Indicators-Incremented'!E2*Metadata!C254)</f>
+        <v>3.5398421531655595</v>
+      </c>
+      <c r="F2" s="20">
+        <f>IF(Metadata!C255&gt;0,'Indicators-Incremented'!F2*Metadata!C255)</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G2" s="20">
+        <f>IF(Metadata!C256&gt;0,'Indicators-Incremented'!G2*Metadata!C256)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="20">
+        <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B3*Metadata!C252)</f>
+        <v>7</v>
+      </c>
+      <c r="C3" s="20">
+        <f>IF(Metadata!C253&gt;0,'Indicators-Incremented'!C3*Metadata!C253)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="20">
+        <f>IF(Metadata!C257&gt;0,'Indicators-Incremented'!D3*Metadata!C257)</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="E3" s="20">
+        <f>IF(Metadata!C254&gt;0,'Indicators-Incremented'!E3*Metadata!C254)</f>
+        <v>3.9281003364321188</v>
+      </c>
+      <c r="F3" s="20">
+        <f>IF(Metadata!C255&gt;0,'Indicators-Incremented'!F3*Metadata!C255)</f>
+        <v>6.8452994616207476</v>
+      </c>
+      <c r="G3" s="20">
+        <f>IF(Metadata!C256&gt;0,'Indicators-Incremented'!G3*Metadata!C256)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="20">
+        <f>IF(Metadata!C252&gt;0,'Indicators-Incremented'!B4*Metadata!C252)</f>
+        <v>9</v>
+      </c>
+      <c r="C4" s="20">
+        <f>IF(Metadata!C253&gt;0,'Indicators-Incremented'!C4*Metadata!C253)</f>
+        <v>4.5</v>
+      </c>
+      <c r="D4" s="20">
+        <f>IF(Metadata!C257&gt;0,'Indicators-Incremented'!D4*Metadata!C257)</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="E4" s="20">
+        <f>IF(Metadata!C254&gt;0,'Indicators-Incremented'!E4*Metadata!C254)</f>
+        <v>4.5320575104023222</v>
+      </c>
+      <c r="F4" s="20">
+        <f>IF(Metadata!C255&gt;0,'Indicators-Incremented'!F4*Metadata!C255)</f>
+        <v>8.5773502691896262</v>
+      </c>
+      <c r="G4" s="20">
+        <f>IF(Metadata!C256&gt;0,'Indicators-Incremented'!G4*Metadata!C256)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A72:A336 A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$252:$A$257</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!B$2:'Indicators-Weighted'!C$2)</f>
+        <v>5.75</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!D2)</f>
+        <v>9.1208970766356092</v>
+      </c>
+      <c r="D2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!E2)</f>
+        <v>3.5398421531655595</v>
+      </c>
+      <c r="E2" s="21">
+        <f>AVERAGE('Indicators-Weighted'!G2:'Indicators-Weighted'!F2)</f>
+        <v>6.0386751345948131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="21">
+        <f>AVERAGE('Indicators-Weighted'!B$3:'Indicators-Weighted'!C$3)</f>
+        <v>5.5</v>
+      </c>
+      <c r="C3" s="21">
+        <f>AVERAGE('Indicators-Weighted'!D3)</f>
+        <v>7.1993592309745642</v>
+      </c>
+      <c r="D3" s="21">
+        <f>AVERAGE('Indicators-Weighted'!E3)</f>
+        <v>3.9281003364321188</v>
+      </c>
+      <c r="E3" s="21">
+        <f>AVERAGE('Indicators-Weighted'!G3:'Indicators-Weighted'!F3)</f>
+        <v>5.4226497308103738</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="21">
+        <f>AVERAGE('Indicators-Weighted'!B$4:'Indicators-Weighted'!C$4)</f>
+        <v>6.75</v>
+      </c>
+      <c r="C4" s="21">
+        <f>AVERAGE('Indicators-Weighted'!D4)</f>
+        <v>7.6797436923898257</v>
+      </c>
+      <c r="D4" s="21">
+        <f>AVERAGE('Indicators-Weighted'!E4)</f>
+        <v>4.5320575104023222</v>
+      </c>
+      <c r="E4" s="21">
+        <f>AVERAGE('Indicators-Weighted'!G4:'Indicators-Weighted'!F4)</f>
+        <v>6.5386751345948131</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$261:$A$264</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:O1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="21">
+        <f>AVERAGE('Components-Weighted'!B2:'Components-Weighted'!C2)</f>
+        <v>7.4354485383178046</v>
+      </c>
+      <c r="C2" s="21">
+        <f>AVERAGE('Components-Weighted'!D2:'Components-Weighted'!E2)</f>
+        <v>4.7892586438801867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="21">
+        <f>AVERAGE('Components-Weighted'!B3:'Components-Weighted'!C3)</f>
+        <v>6.3496796154872825</v>
+      </c>
+      <c r="C3" s="21">
+        <f>AVERAGE('Components-Weighted'!D3:'Components-Weighted'!E3)</f>
+        <v>4.6753750336212461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="21">
+        <f>AVERAGE('Components-Weighted'!B4:'Components-Weighted'!C4)</f>
+        <v>7.2148718461949128</v>
+      </c>
+      <c r="C4" s="21">
+        <f>AVERAGE('Components-Weighted'!D4:'Components-Weighted'!E4)</f>
+        <v>5.5353663224985681</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Metadata!$A$267:$A$268</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:C1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2">
+        <f>'Subindex-Weighted'!B2*Metadata!B267+'Subindex-Weighted'!C2*Metadata!B268</f>
+        <v>5.8477346016552341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <f>'Subindex-Weighted'!B3*Metadata!B267+'Subindex-Weighted'!C3*Metadata!B268</f>
+        <v>5.3450968663676601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <f>'Subindex-Weighted'!B4*Metadata!B267+'Subindex-Weighted'!C4*Metadata!B268</f>
+        <v>6.2071685319771062</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G2" t="s">
+        <v>273</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="22">
+        <f>RANK('Components-Weighted'!B2,'Components-Weighted'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="22">
+        <f>RANK('Components-Weighted'!C2,'Components-Weighted'!C$2:C$4)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="22">
+        <f>RANK('Subindex-Weighted'!B2,'Subindex-Weighted'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <f>RANK('Components-Weighted'!D2,'Components-Weighted'!D$2:D$4)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="22">
+        <f>RANK('Components-Weighted'!E2,'Components-Weighted'!E$2:E$4)</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="22">
+        <f>RANK('Subindex-Weighted'!C2,'Subindex-Weighted'!C$2:C$4)</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="24">
+        <f>RANK('Index-Weighted'!B2,'Index-Weighted'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="22">
+        <f>RANK('Components-Weighted'!B3,'Components-Weighted'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="22">
+        <f>RANK('Components-Weighted'!C3,'Components-Weighted'!C$2:C$4)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="22">
+        <f>RANK('Subindex-Weighted'!B3,'Subindex-Weighted'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+      <c r="E4" s="22">
+        <f>RANK('Components-Weighted'!D3,'Components-Weighted'!D$2:D$4)</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="22">
+        <f>RANK('Components-Weighted'!E3,'Components-Weighted'!E$2:E$4)</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="22">
+        <f>RANK('Subindex-Weighted'!C3,'Subindex-Weighted'!C$2:C$4)</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="24">
+        <f>RANK('Index-Weighted'!B3,'Index-Weighted'!B$2:B$4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="22">
+        <f>RANK('Components-Weighted'!B4,'Components-Weighted'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="22">
+        <f>RANK('Components-Weighted'!C4,'Components-Weighted'!C$2:C$4)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="22">
+        <f>RANK('Subindex-Weighted'!B4,'Subindex-Weighted'!B$2:B$4)</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="22">
+        <f>RANK('Components-Weighted'!D4,'Components-Weighted'!D$2:D$4)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <f>RANK('Components-Weighted'!E4,'Components-Weighted'!E$2:E$4)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="22">
+        <f>RANK('Subindex-Weighted'!C4,'Subindex-Weighted'!C$2:C$4)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="24">
+        <f>RANK('Index-Weighted'!B4,'Index-Weighted'!B$2:B$4)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2009</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2010</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
       <c r="B4" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -2845,8 +4947,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
+      <c r="A6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>5</v>
@@ -2859,16 +4961,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
         <v>4</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>4</v>
       </c>
     </row>
@@ -2894,7 +4996,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2906,15 +5008,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -2922,7 +5024,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -2936,15 +5038,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -2958,30 +5060,30 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
+      <c r="A6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E6" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
         <v>6</v>
       </c>
       <c r="D7" s="5">
         <v>8</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -3005,7 +5107,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3017,15 +5119,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -3033,7 +5135,7 @@
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2009</v>
@@ -3047,15 +5149,15 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3069,8 +5171,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
+      <c r="A6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -3083,16 +5185,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
         <v>4</v>
       </c>
       <c r="D7" s="5">
         <v>6</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>8</v>
       </c>
     </row>
@@ -3115,10 +5217,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3130,15 +5232,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -3146,7 +5248,7 @@
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -3154,15 +5256,15 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
@@ -3170,19 +5272,37 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
+      <c r="A6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3207,7 +5327,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3219,23 +5339,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
         <v>2011</v>
@@ -3243,35 +5363,38 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>7</v>
+        <f>('Q1'!C$5-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
+      <c r="A6" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="5">
-        <v>3</v>
+        <f>('Q1'!C$6-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
-        <v>4</v>
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('Q1'!C$7-'Q1'!C$9)/'Q1'!C$10</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3293,10 +5416,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3306,197 +5429,79 @@
     <col min="3" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5">
-        <v>5</v>
-      </c>
-      <c r="E7" s="14">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
-      <formula1>countries</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>datatype</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>indicators</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="5"/>
-    <col min="2" max="2" width="9" style="9"/>
-    <col min="3" max="16384" width="9" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" s="5">
+        <f>AVERAGE(C5:C7)</f>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2009</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2010</v>
-      </c>
-      <c r="E3" s="6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="14">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5">
-        <v>8</v>
-      </c>
-      <c r="E7" s="18">
-        <v>10</v>
+      <c r="C10" s="5">
+        <f>STDEV(C5:C7)</f>
+        <v>2.0816659994661335</v>
       </c>
     </row>
   </sheetData>
@@ -3514,4 +5519,96 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="9" style="9"/>
+    <col min="3" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5">
+        <f>('Q2'!C$5-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>1.1208970766356094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5">
+        <f>('Q2'!C$6-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.80064076902543546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5">
+        <f>('Q2'!C$7-'Q2'!C$9)/'Q2'!C$10</f>
+        <v>-0.32025630761017432</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>indicators</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>datatype</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1048576">
+      <formula1>countries</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>